<commit_message>
Made buttons pretty, fixed a persistence issue.
</commit_message>
<xml_diff>
--- a/Bescreweled-Regression-Test 013012.xlsx
+++ b/Bescreweled-Regression-Test 013012.xlsx
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>CO-11</t>
-  </si>
-  <si>
-    <t>Adjacent code is better, watch 2nd and 3rd 5 Rage in successive iterations.</t>
   </si>
 </sst>
 </file>
@@ -210,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -324,6 +321,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -500,6 +512,21 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -507,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -525,10 +552,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -537,7 +564,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -549,42 +576,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -594,16 +624,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <condense val="0"/>
@@ -625,18 +657,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -932,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -947,7 +967,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
@@ -1031,7 +1051,7 @@
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="33" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="10"/>
@@ -1045,7 +1065,7 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="34" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="9"/>
@@ -1085,7 +1105,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="120">
+    <row r="10" spans="1:6" ht="120.75" thickBot="1">
       <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -1099,42 +1119,38 @@
       <c r="E10" s="9"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" ht="150.75" thickBot="1">
-      <c r="A11" s="34"/>
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:6" ht="151.5" thickTop="1" thickBot="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
@@ -1166,16 +1182,16 @@
     </row>
     <row r="15" spans="1:6" ht="31.5" thickTop="1" thickBot="1">
       <c r="A15" s="12"/>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="36" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>